<commit_message>
membuat PCB LEGI versi HALIM dengan komunikasi LoRa
</commit_message>
<xml_diff>
--- a/pengajuan monKWH-HALIM.xlsx
+++ b/pengajuan monKWH-HALIM.xlsx
@@ -263,19 +263,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -560,11 +563,12 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="3.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
@@ -597,7 +601,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -606,13 +610,13 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>469</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <v>10000</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="4">
         <f>(C2*D2)+E2</f>
         <v>10469</v>
       </c>
@@ -621,19 +625,22 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>6000</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>10000</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <f t="shared" ref="F3:F24" si="0">(C3*D3)+E3</f>
         <v>16000</v>
       </c>
@@ -642,17 +649,20 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
       <c r="B4" t="s">
         <v>45</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>1700</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5">
+      <c r="E4" s="4"/>
+      <c r="F4" s="4">
         <f t="shared" si="0"/>
         <v>3400</v>
       </c>
@@ -661,17 +671,20 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
       <c r="B5" t="s">
         <v>50</v>
       </c>
       <c r="C5">
         <v>5</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>300</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5">
+      <c r="E5" s="4"/>
+      <c r="F5" s="4">
         <f t="shared" si="0"/>
         <v>1500</v>
       </c>
@@ -680,17 +693,20 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
       <c r="B6" t="s">
         <v>52</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>1800</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5">
+      <c r="E6" s="4"/>
+      <c r="F6" s="4">
         <f t="shared" si="0"/>
         <v>1800</v>
       </c>
@@ -699,17 +715,20 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
       <c r="B7" t="s">
         <v>54</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>3400</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5">
+      <c r="E7" s="4"/>
+      <c r="F7" s="4">
         <f t="shared" si="0"/>
         <v>3400</v>
       </c>
@@ -718,19 +737,22 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
       <c r="C8">
         <v>10</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>500</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>10000</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <f t="shared" si="0"/>
         <v>15000</v>
       </c>
@@ -739,17 +761,20 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
       <c r="B9" t="s">
         <v>15</v>
       </c>
       <c r="C9">
         <v>10</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>500</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5">
+      <c r="E9" s="4"/>
+      <c r="F9" s="4">
         <f t="shared" si="0"/>
         <v>5000</v>
       </c>
@@ -758,17 +783,20 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
       <c r="B10" t="s">
         <v>16</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>3050</v>
       </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5">
+      <c r="E10" s="4"/>
+      <c r="F10" s="4">
         <f t="shared" si="0"/>
         <v>3050</v>
       </c>
@@ -777,19 +805,22 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
       <c r="B11" t="s">
         <v>18</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>100</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <v>20000</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <f t="shared" si="0"/>
         <v>20200</v>
       </c>
@@ -798,19 +829,22 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
       <c r="B12" t="s">
         <v>21</v>
       </c>
       <c r="C12">
         <v>10</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>500</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="4">
         <v>20000</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="4">
         <f t="shared" si="0"/>
         <v>25000</v>
       </c>
@@ -819,19 +853,22 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
       <c r="B13" t="s">
         <v>22</v>
       </c>
       <c r="C13">
         <v>10</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>600</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="4">
         <v>20000</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="4">
         <f t="shared" si="0"/>
         <v>26000</v>
       </c>
@@ -840,23 +877,26 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
       <c r="B14" t="s">
         <v>24</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>1000</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="4">
         <v>20000</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="4">
         <f t="shared" si="0"/>
         <v>21000</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="6" t="s">
         <v>30</v>
       </c>
       <c r="H14" s="2" t="s">
@@ -864,57 +904,66 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
       <c r="B15" t="s">
         <v>26</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <v>1000</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5">
+      <c r="E15" s="4"/>
+      <c r="F15" s="4">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="G15" s="3"/>
+      <c r="G15" s="6"/>
       <c r="H15" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="5">
+        <v>15</v>
+      </c>
       <c r="B16" t="s">
         <v>29</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="4">
         <v>1000</v>
       </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5">
+      <c r="E16" s="4"/>
+      <c r="F16" s="4">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="G16" s="3"/>
+      <c r="G16" s="6"/>
       <c r="H16" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="4" t="s">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="5">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C17">
         <v>5</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="4">
         <v>300</v>
       </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5">
+      <c r="E17" s="4"/>
+      <c r="F17" s="4">
         <f t="shared" si="0"/>
         <v>1500</v>
       </c>
@@ -922,18 +971,21 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="4" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="5">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>37</v>
       </c>
       <c r="C18">
         <v>2</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="4">
         <v>1200</v>
       </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5">
+      <c r="E18" s="4"/>
+      <c r="F18" s="4">
         <f t="shared" si="0"/>
         <v>2400</v>
       </c>
@@ -941,20 +993,23 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="5">
+        <v>18</v>
+      </c>
       <c r="B19" t="s">
         <v>33</v>
       </c>
       <c r="C19">
         <v>2</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="4">
         <v>2000</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="4">
         <v>20000</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F19" s="4">
         <f t="shared" si="0"/>
         <v>24000</v>
       </c>
@@ -962,20 +1017,23 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="5">
+        <v>19</v>
+      </c>
       <c r="B20" t="s">
         <v>36</v>
       </c>
       <c r="C20">
         <v>10</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="4">
         <v>299</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="4">
         <v>20000</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20" s="4">
         <f t="shared" si="0"/>
         <v>22990</v>
       </c>
@@ -983,20 +1041,23 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="5">
+        <v>20</v>
+      </c>
       <c r="B21" t="s">
         <v>40</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="4">
         <v>41750</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="4">
         <v>10000</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F21" s="4">
         <f t="shared" si="0"/>
         <v>51750</v>
       </c>
@@ -1004,20 +1065,23 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="5">
+        <v>21</v>
+      </c>
       <c r="B22" t="s">
         <v>41</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="4">
         <v>80000</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="4">
         <v>10000</v>
       </c>
-      <c r="F22" s="5">
+      <c r="F22" s="4">
         <f t="shared" si="0"/>
         <v>90000</v>
       </c>
@@ -1025,18 +1089,21 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="5">
+        <v>22</v>
+      </c>
       <c r="B23" t="s">
         <v>44</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="4">
         <v>3500</v>
       </c>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5">
+      <c r="E23" s="4"/>
+      <c r="F23" s="4">
         <f t="shared" si="0"/>
         <v>3500</v>
       </c>
@@ -1044,18 +1111,21 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="5">
+        <v>23</v>
+      </c>
       <c r="B24" t="s">
         <v>47</v>
       </c>
       <c r="C24">
         <v>3</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="4">
         <v>15000</v>
       </c>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5">
+      <c r="E24" s="4"/>
+      <c r="F24" s="4">
         <f t="shared" si="0"/>
         <v>45000</v>
       </c>

</xml_diff>